<commit_message>
Generate wordclouds for NER
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/social_media/Fakespeak_social_media_named_entities_frequency.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/social_media/Fakespeak_social_media_named_entities_frequency.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>Entity</t>
   </si>
@@ -34,18 +34,57 @@
     <t>Count</t>
   </si>
   <si>
+    <t>infrastructure</t>
+  </si>
+  <si>
+    <t>invoice</t>
+  </si>
+  <si>
+    <t>receivership</t>
+  </si>
+  <si>
+    <t>economy</t>
+  </si>
+  <si>
     <t>United States of America</t>
   </si>
   <si>
+    <t>repair</t>
+  </si>
+  <si>
     <t>bridge</t>
   </si>
   <si>
     <t>Michigan</t>
   </si>
   <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>pork</t>
+  </si>
+  <si>
     <t>Democratic Party</t>
   </si>
   <si>
+    <t>productivity</t>
+  </si>
+  <si>
+    <t>hundred</t>
+  </si>
+  <si>
+    <t>global warming</t>
+  </si>
+  <si>
+    <t>American Capitalism</t>
+  </si>
+  <si>
+    <t>agenda</t>
+  </si>
+  <si>
     <t>First Step</t>
   </si>
   <si>
@@ -58,27 +97,90 @@
     <t>Houston Texans</t>
   </si>
   <si>
+    <t>act</t>
+  </si>
+  <si>
+    <t>Immediately</t>
+  </si>
+  <si>
+    <t>2012 VP113</t>
+  </si>
+  <si>
     <t>Texas</t>
   </si>
   <si>
+    <t>illegal immigration</t>
+  </si>
+  <si>
+    <t>generation</t>
+  </si>
+  <si>
+    <t>ORG</t>
+  </si>
+  <si>
     <t>GPE</t>
   </si>
   <si>
+    <t>PERCENT</t>
+  </si>
+  <si>
     <t>NORP</t>
   </si>
   <si>
+    <t>CARDINAL</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q121359</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q190581</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q474341</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q159810</t>
+  </si>
+  <si>
     <t>https://www.wikidata.org/wiki/Q30</t>
   </si>
   <si>
+    <t>https://www.wikidata.org/wiki/Q2144962</t>
+  </si>
+  <si>
     <t>https://www.wikidata.org/wiki/Q12280</t>
   </si>
   <si>
     <t>https://www.wikidata.org/wiki/Q1166</t>
   </si>
   <si>
+    <t>https://www.wikidata.org/wiki/Q34442</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q11229</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q191768</t>
+  </si>
+  <si>
     <t>https://www.wikidata.org/wiki/Q29552</t>
   </si>
   <si>
+    <t>https://www.wikidata.org/wiki/Q2111958</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q313354</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q7942</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q4743290</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q1758159</t>
+  </si>
+  <si>
     <t>https://www.wikidata.org/wiki/Q3269975</t>
   </si>
   <si>
@@ -91,22 +193,73 @@
     <t>https://www.wikidata.org/wiki/Q223514</t>
   </si>
   <si>
+    <t>https://www.wikidata.org/wiki/Q820655</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q6004788</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q15980607</t>
+  </si>
+  <si>
     <t>https://www.wikidata.org/wiki/Q1439</t>
   </si>
   <si>
+    <t>https://www.wikidata.org/wiki/Q856681</t>
+  </si>
+  <si>
+    <t>https://www.wikidata.org/wiki/Q213381</t>
+  </si>
+  <si>
+    <t>bill</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
     <t>America</t>
   </si>
   <si>
+    <t>repairs</t>
+  </si>
+  <si>
     <t>bridges</t>
   </si>
   <si>
+    <t>roads</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
     <t>Democrats</t>
   </si>
   <si>
+    <t>hundreds</t>
+  </si>
+  <si>
+    <t>climate change</t>
+  </si>
+  <si>
+    <t>American capitalism</t>
+  </si>
+  <si>
     <t>first step</t>
   </si>
   <si>
     <t>Texans</t>
+  </si>
+  <si>
+    <t>IMMEDIATELY</t>
+  </si>
+  <si>
+    <t>Biden</t>
+  </si>
+  <si>
+    <t>illegal immigrants</t>
+  </si>
+  <si>
+    <t>generations</t>
   </si>
 </sst>
 </file>
@@ -477,7 +630,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -507,20 +660,17 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
       <c r="C2">
-        <v>30</v>
+        <v>121359</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -528,16 +678,16 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>12280</v>
+        <v>190581</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -545,16 +695,16 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>1166</v>
+        <v>474341</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -564,17 +714,14 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5">
-        <v>29552</v>
+        <v>159810</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -584,14 +731,17 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
       <c r="C6">
-        <v>3269975</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -602,13 +752,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>2068307</v>
+        <v>2144962</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -619,13 +769,13 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>846570</v>
+        <v>12280</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -636,16 +786,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C9">
-        <v>223514</v>
+        <v>1166</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -655,19 +805,343 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10">
+        <v>34442</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>11229</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>191768</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>29552</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>2111958</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>313354</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>7942</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>4743290</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>1758159</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>3269975</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>2068307</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>846570</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>223514</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <v>820655</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>6004788</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <v>15980607</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26">
         <v>1439</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10">
+      <c r="D26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>856681</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>213381</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28">
         <v>1</v>
       </c>
     </row>
@@ -682,6 +1156,24 @@
     <hyperlink ref="D8" r:id="rId7"/>
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix problems with wordclouds
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/social_media/Fakespeak_social_media_named_entities_frequency.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/social_media/Fakespeak_social_media_named_entities_frequency.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Entity</t>
   </si>
@@ -34,87 +34,36 @@
     <t>Count</t>
   </si>
   <si>
-    <t>infrastructure</t>
-  </si>
-  <si>
-    <t>invoice</t>
-  </si>
-  <si>
     <t>receivership</t>
   </si>
   <si>
-    <t>economy</t>
-  </si>
-  <si>
     <t>United States of America</t>
   </si>
   <si>
-    <t>repair</t>
-  </si>
-  <si>
-    <t>bridge</t>
-  </si>
-  <si>
     <t>Michigan</t>
   </si>
   <si>
-    <t>road</t>
-  </si>
-  <si>
     <t>percent</t>
   </si>
   <si>
-    <t>pork</t>
-  </si>
-  <si>
     <t>Democratic Party</t>
   </si>
   <si>
-    <t>productivity</t>
-  </si>
-  <si>
     <t>hundred</t>
   </si>
   <si>
-    <t>global warming</t>
-  </si>
-  <si>
-    <t>American Capitalism</t>
-  </si>
-  <si>
-    <t>agenda</t>
-  </si>
-  <si>
-    <t>First Step</t>
-  </si>
-  <si>
-    <t>Green New Deal</t>
-  </si>
-  <si>
     <t>Americans</t>
   </si>
   <si>
     <t>Houston Texans</t>
   </si>
   <si>
-    <t>act</t>
-  </si>
-  <si>
-    <t>Immediately</t>
-  </si>
-  <si>
     <t>2012 VP113</t>
   </si>
   <si>
     <t>Texas</t>
   </si>
   <si>
-    <t>illegal immigration</t>
-  </si>
-  <si>
-    <t>generation</t>
-  </si>
-  <si>
     <t>ORG</t>
   </si>
   <si>
@@ -130,105 +79,42 @@
     <t>CARDINAL</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q121359</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q190581</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q474341</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q159810</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q30</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q2144962</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q12280</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q1166</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q34442</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q11229</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q191768</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q29552</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q2111958</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q313354</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q7942</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q4743290</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q1758159</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q3269975</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q2068307</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q846570</t>
   </si>
   <si>
     <t>https://www.wikidata.org/wiki/Q223514</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q820655</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q6004788</t>
-  </si>
-  <si>
     <t>https://www.wikidata.org/wiki/Q15980607</t>
   </si>
   <si>
     <t>https://www.wikidata.org/wiki/Q1439</t>
   </si>
   <si>
-    <t>https://www.wikidata.org/wiki/Q856681</t>
-  </si>
-  <si>
-    <t>https://www.wikidata.org/wiki/Q213381</t>
-  </si>
-  <si>
-    <t>bill</t>
-  </si>
-  <si>
     <t>Administration</t>
   </si>
   <si>
     <t>America</t>
   </si>
   <si>
-    <t>repairs</t>
-  </si>
-  <si>
-    <t>bridges</t>
-  </si>
-  <si>
-    <t>roads</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -238,28 +124,10 @@
     <t>hundreds</t>
   </si>
   <si>
-    <t>climate change</t>
-  </si>
-  <si>
-    <t>American capitalism</t>
-  </si>
-  <si>
-    <t>first step</t>
-  </si>
-  <si>
     <t>Texans</t>
   </si>
   <si>
-    <t>IMMEDIATELY</t>
-  </si>
-  <si>
     <t>Biden</t>
-  </si>
-  <si>
-    <t>illegal immigrants</t>
-  </si>
-  <si>
-    <t>generations</t>
   </si>
 </sst>
 </file>
@@ -630,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -660,34 +528,40 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
       <c r="C2">
-        <v>121359</v>
+        <v>474341</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
       <c r="C3">
-        <v>190581</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -695,16 +569,16 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>474341</v>
+        <v>1166</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -714,14 +588,17 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
       <c r="C5">
-        <v>159810</v>
+        <v>11229</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -732,16 +609,16 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>29552</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
         <v>34</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>67</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -751,14 +628,17 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
       <c r="C7">
-        <v>2144962</v>
+        <v>313354</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -768,14 +648,17 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
       <c r="C8">
-        <v>12280</v>
+        <v>846570</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -786,16 +669,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>1166</v>
+        <v>223514</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -805,14 +688,17 @@
       <c r="A10" t="s">
         <v>14</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
       <c r="C10">
-        <v>34442</v>
+        <v>15980607</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -823,325 +709,18 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>11229</v>
+        <v>1439</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>191768</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13">
-        <v>29552</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>2111958</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15">
-        <v>313354</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>7942</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>4743290</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18">
-        <v>1758159</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19">
-        <v>3269975</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>2068307</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21">
-        <v>846570</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22">
-        <v>223514</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <v>820655</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24">
-        <v>6004788</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25">
-        <v>15980607</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26">
-        <v>1439</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27">
-        <v>856681</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28">
-        <v>213381</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28">
         <v>1</v>
       </c>
     </row>
@@ -1157,23 +736,6 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D20" r:id="rId19"/>
-    <hyperlink ref="D21" r:id="rId20"/>
-    <hyperlink ref="D22" r:id="rId21"/>
-    <hyperlink ref="D23" r:id="rId22"/>
-    <hyperlink ref="D24" r:id="rId23"/>
-    <hyperlink ref="D25" r:id="rId24"/>
-    <hyperlink ref="D26" r:id="rId25"/>
-    <hyperlink ref="D27" r:id="rId26"/>
-    <hyperlink ref="D28" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>